<commit_message>
Auditoria Carta de Aceptación
Resultados Auditoria Carta de Aceptación
</commit_message>
<xml_diff>
--- a/Proyectos/Viaticos/05. Calidad/Viaticos-Auditoria.xlsx
+++ b/Proyectos/Viaticos/05. Calidad/Viaticos-Auditoria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19230" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19230" windowHeight="7665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="167">
   <si>
     <t>Checklist de Auditorías</t>
   </si>
@@ -426,9 +426,6 @@
     <t>¿Se tiene la lista de entregables?</t>
   </si>
   <si>
-    <t>¿Se tiene firmada la carta de aceptación?</t>
-  </si>
-  <si>
     <t>¿Se tienen los datos del cliente?</t>
   </si>
   <si>
@@ -540,9 +537,6 @@
     <t>¿Se generó una estimación el proyecto?</t>
   </si>
   <si>
-    <t>Mayra Tejeda</t>
-  </si>
-  <si>
     <t>No está definido un estatus para las pruebas</t>
   </si>
   <si>
@@ -550,6 +544,12 @@
   </si>
   <si>
     <t>¿Se identificó el responsable para las pruebas?</t>
+  </si>
+  <si>
+    <t>Jovanny Zepeda</t>
+  </si>
+  <si>
+    <t>Se sugiere ampliar los datos del cliente</t>
   </si>
 </sst>
 </file>
@@ -963,7 +963,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1216,28 +1216,31 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1246,35 +1249,7 @@
     <cellStyle name="Normal 3" xfId="1"/>
     <cellStyle name="Porcentaje 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1413,11 +1388,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="63590400"/>
-        <c:axId val="63591936"/>
+        <c:axId val="106120320"/>
+        <c:axId val="106121856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63590400"/>
+        <c:axId val="106120320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,14 +1433,14 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63591936"/>
+        <c:crossAx val="106121856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63591936"/>
+        <c:axId val="106121856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1515,7 +1490,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63590400"/>
+        <c:crossAx val="106120320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1557,7 +1532,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1598,7 +1573,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1675,7 +1649,7 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1691,11 +1665,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="62555648"/>
-        <c:axId val="62557184"/>
+        <c:axId val="109986944"/>
+        <c:axId val="109988864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62555648"/>
+        <c:axId val="109986944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,14 +1710,14 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62557184"/>
+        <c:crossAx val="109988864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62557184"/>
+        <c:axId val="109988864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1793,7 +1767,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62555648"/>
+        <c:crossAx val="109986944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1835,7 +1809,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1871,7 +1845,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1940,11 +1913,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="104409728"/>
-        <c:axId val="104423808"/>
+        <c:axId val="120101120"/>
+        <c:axId val="107393024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104409728"/>
+        <c:axId val="120101120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1985,14 +1958,14 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104423808"/>
+        <c:crossAx val="107393024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104423808"/>
+        <c:axId val="107393024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2042,7 +2015,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104409728"/>
+        <c:crossAx val="120101120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2084,7 +2057,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2120,7 +2093,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2189,11 +2161,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="104456192"/>
-        <c:axId val="104457728"/>
+        <c:axId val="107412864"/>
+        <c:axId val="108663936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104456192"/>
+        <c:axId val="107412864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,14 +2206,14 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104457728"/>
+        <c:crossAx val="108663936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104457728"/>
+        <c:axId val="108663936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2291,7 +2263,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="104456192"/>
+        <c:crossAx val="107412864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2333,7 +2305,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2982,7 +2954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2992,7 +2964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3032,10 +3004,10 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="78" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6" s="79"/>
       <c r="E6" s="79"/>
@@ -3046,7 +3018,7 @@
         <v>66</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D7" s="82"/>
       <c r="E7" s="82"/>
@@ -3057,7 +3029,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="84">
-        <v>42472</v>
+        <v>42474</v>
       </c>
       <c r="D8" s="85"/>
       <c r="E8" s="85"/>
@@ -3068,7 +3040,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="85"/>
       <c r="E9" s="85"/>
@@ -3078,7 +3050,7 @@
     <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="B12" s="73" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" s="73"/>
       <c r="D12" s="73"/>
@@ -3167,7 +3139,7 @@
     <row r="19" spans="2:8" ht="16.5" customHeight="1"/>
     <row r="20" spans="2:8" ht="16.5" customHeight="1">
       <c r="B20" s="73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="73"/>
       <c r="D20" s="73"/>
@@ -3259,32 +3231,32 @@
         <v>Carta de Aceptación</v>
       </c>
       <c r="C27" s="9">
-        <f>COUNTA(Productos!D72:D75)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="10" t="e">
-        <f>COUNTIF((Productos!D72:D75),"x")/(COUNTIF((Productos!D72:D75),"x")+COUNTIF((Productos!E72:E75),"x"))</f>
-        <v>#DIV/0!</v>
+        <f>COUNTA(Productos!D72:D74)</f>
+        <v>3</v>
+      </c>
+      <c r="D27" s="10">
+        <f>COUNTIF((Productos!D72:D74),"x")/(COUNTIF((Productos!D72:D74),"x")+COUNTIF((Productos!E72:E74),"x"))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="16.5" customHeight="1">
       <c r="B28" s="8" t="str">
-        <f>Productos!B77</f>
+        <f>Productos!B76</f>
         <v>Reporte de Monitoreo</v>
       </c>
       <c r="C28" s="9">
-        <f>COUNTA(Productos!D78:D84)</f>
+        <f>COUNTA(Productos!D77:D83)</f>
         <v>0</v>
       </c>
       <c r="D28" s="10" t="e">
-        <f>COUNTIF((Productos!D78:D84),"x")/(COUNTIF((Productos!D78:D84),"x")+COUNTIF((Productos!E78:E84),"x"))</f>
+        <f>COUNTIF((Productos!D77:D83),"x")/(COUNTIF((Productos!D77:D83),"x")+COUNTIF((Productos!E77:E83),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="19.5" customHeight="1"/>
     <row r="30" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="B30" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C30" s="75"/>
       <c r="D30" s="75"/>
@@ -3440,7 +3412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -3464,22 +3436,22 @@
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:7" ht="21" customHeight="1">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="92"/>
+      <c r="D3" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88" t="s">
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1">
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="53" t="s">
         <v>12</v>
       </c>
@@ -3489,17 +3461,17 @@
       <c r="F4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="88"/>
+      <c r="G4" s="92"/>
     </row>
     <row r="5" spans="2:7" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B6" s="20">
@@ -3509,7 +3481,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
@@ -3524,7 +3496,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
@@ -3539,7 +3511,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
@@ -3554,7 +3526,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
@@ -3569,7 +3541,7 @@
         <v>76</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -3584,7 +3556,7 @@
         <v>77</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
@@ -3592,14 +3564,14 @@
     </row>
     <row r="12" spans="2:7" s="24" customFormat="1" ht="16.5"/>
     <row r="13" spans="2:7" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="93"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
     </row>
     <row r="14" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B14" s="20">
@@ -3609,7 +3581,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -3624,7 +3596,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
@@ -3639,7 +3611,7 @@
         <v>80</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
@@ -3654,7 +3626,7 @@
         <v>81</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
@@ -3669,7 +3641,7 @@
         <v>82</v>
       </c>
       <c r="D18" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -3684,7 +3656,7 @@
         <v>83</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
@@ -3696,10 +3668,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D20" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
@@ -3707,14 +3679,14 @@
     </row>
     <row r="21" spans="2:7" s="24" customFormat="1" ht="16.5"/>
     <row r="22" spans="2:7" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="93"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
     </row>
     <row r="23" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B23" s="20">
@@ -3724,7 +3696,7 @@
         <v>84</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
@@ -3732,14 +3704,14 @@
     </row>
     <row r="24" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B24" s="20">
-        <f>+B23+1</f>
+        <f t="shared" ref="B24:B30" si="2">+B23+1</f>
         <v>2</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>85</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
@@ -3747,14 +3719,14 @@
     </row>
     <row r="25" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B25" s="20">
-        <f>+B24+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>86</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -3762,14 +3734,14 @@
     </row>
     <row r="26" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B26" s="20">
-        <f>+B25+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>87</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -3777,14 +3749,14 @@
     </row>
     <row r="27" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B27" s="20">
-        <f>+B26+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>88</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
@@ -3792,14 +3764,14 @@
     </row>
     <row r="28" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B28" s="20">
-        <f>+B27+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>91</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
@@ -3807,14 +3779,14 @@
     </row>
     <row r="29" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B29" s="20">
-        <f>+B28+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>89</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
@@ -3822,14 +3794,14 @@
     </row>
     <row r="30" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B30" s="20">
-        <f>+B29+1</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>90</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
@@ -3837,10 +3809,10 @@
     </row>
     <row r="31" spans="2:7" s="24" customFormat="1" ht="16.5"/>
     <row r="32" spans="2:7" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="B32" s="91" t="s">
+      <c r="B32" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="91"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
@@ -3851,7 +3823,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -3864,7 +3836,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
@@ -3873,7 +3845,7 @@
     </row>
     <row r="35" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B35" s="20">
-        <f t="shared" ref="B35:B36" si="2">+B34+1</f>
+        <f t="shared" ref="B35:B36" si="3">+B34+1</f>
         <v>3</v>
       </c>
       <c r="C35" s="21" t="s">
@@ -3886,11 +3858,11 @@
     </row>
     <row r="36" spans="2:7" s="24" customFormat="1" ht="16.5">
       <c r="B36" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -3899,14 +3871,14 @@
     </row>
     <row r="37" spans="2:7" s="24" customFormat="1" ht="16.5"/>
     <row r="38" spans="2:7" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="B38" s="91" t="s">
+      <c r="B38" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="91"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="91"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="88"/>
+      <c r="F38" s="88"/>
+      <c r="G38" s="88"/>
     </row>
     <row r="39" spans="2:7" s="24" customFormat="1" ht="17.25" customHeight="1">
       <c r="B39" s="20">
@@ -3935,7 +3907,7 @@
     </row>
     <row r="41" spans="2:7" s="24" customFormat="1" ht="17.25" customHeight="1">
       <c r="B41" s="20">
-        <f t="shared" ref="B41:B43" si="3">B40+1</f>
+        <f t="shared" ref="B41:B43" si="4">B40+1</f>
         <v>3</v>
       </c>
       <c r="C41" s="21" t="s">
@@ -3948,7 +3920,7 @@
     </row>
     <row r="42" spans="2:7" s="24" customFormat="1" ht="17.25" customHeight="1">
       <c r="B42" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="C42" s="21" t="s">
@@ -3961,11 +3933,11 @@
     </row>
     <row r="43" spans="2:7" s="24" customFormat="1" ht="17.25" customHeight="1">
       <c r="B43" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -3978,6 +3950,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
@@ -3988,15 +3966,9 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="D23:F30 C29:C30">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>IF($D$32,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4008,10 +3980,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -4036,23 +4008,23 @@
     </row>
     <row r="3" spans="1:7" s="35" customFormat="1" ht="17.25" customHeight="1">
       <c r="A3" s="34"/>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="92"/>
+      <c r="D3" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88" t="s">
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="35" customFormat="1" ht="17.25" customHeight="1">
       <c r="A4" s="34"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="53" t="s">
         <v>12</v>
       </c>
@@ -4062,18 +4034,18 @@
       <c r="F4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="88"/>
+      <c r="G4" s="92"/>
     </row>
     <row r="5" spans="1:7" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="28"/>
-      <c r="B5" s="90" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="B5" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A6" s="32"/>
@@ -4084,7 +4056,7 @@
         <v>97</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
@@ -4100,7 +4072,7 @@
         <v>98</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
@@ -4116,7 +4088,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="39"/>
       <c r="F8" s="39"/>
@@ -4129,10 +4101,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="39"/>
       <c r="F9" s="39"/>
@@ -4148,7 +4120,7 @@
         <v>100</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
@@ -4164,7 +4136,7 @@
         <v>101</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
@@ -4177,10 +4149,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
@@ -4196,7 +4168,7 @@
         <v>102</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
@@ -4209,10 +4181,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
@@ -4228,7 +4200,7 @@
         <v>103</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
@@ -4259,14 +4231,14 @@
     </row>
     <row r="18" spans="1:7" s="44" customFormat="1" ht="16.5" customHeight="1">
       <c r="A18" s="43"/>
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
+      <c r="G18" s="91"/>
     </row>
     <row r="19" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A19" s="32"/>
@@ -4274,10 +4246,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
@@ -4290,10 +4262,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="39"/>
@@ -4306,10 +4278,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="39"/>
@@ -4322,10 +4294,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="39"/>
@@ -4338,10 +4310,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="39"/>
       <c r="F23" s="39"/>
@@ -4354,10 +4326,10 @@
         <v>6</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39"/>
@@ -4373,7 +4345,7 @@
         <v>105</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E25" s="39"/>
       <c r="F25" s="39"/>
@@ -4389,7 +4361,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E26" s="39"/>
       <c r="F26" s="39"/>
@@ -4405,7 +4377,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39"/>
@@ -4421,7 +4393,7 @@
         <v>108</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39"/>
@@ -4437,7 +4409,7 @@
         <v>109</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
@@ -4450,10 +4422,10 @@
         <v>12</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="39"/>
@@ -4469,7 +4441,7 @@
         <v>110</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E31" s="39"/>
       <c r="F31" s="39"/>
@@ -4486,14 +4458,14 @@
     </row>
     <row r="33" spans="1:7" s="44" customFormat="1" ht="16.5" customHeight="1">
       <c r="A33" s="43"/>
-      <c r="B33" s="90" t="s">
+      <c r="B33" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="90"/>
-      <c r="G33" s="90"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91"/>
     </row>
     <row r="34" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A34" s="32"/>
@@ -4504,7 +4476,7 @@
         <v>111</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
@@ -4520,7 +4492,7 @@
         <v>112</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
@@ -4536,7 +4508,7 @@
         <v>113</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -4552,7 +4524,7 @@
         <v>114</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
@@ -4568,7 +4540,7 @@
         <v>115</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
@@ -4584,7 +4556,7 @@
         <v>116</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
@@ -4600,7 +4572,7 @@
         <v>20</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
@@ -4616,7 +4588,7 @@
         <v>21</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
@@ -4629,10 +4601,10 @@
         <v>9</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
@@ -4649,11 +4621,11 @@
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="33" customFormat="1" ht="16.5">
@@ -4666,7 +4638,7 @@
         <v>118</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
@@ -4683,14 +4655,14 @@
     </row>
     <row r="46" spans="1:7" s="44" customFormat="1" ht="16.5" customHeight="1">
       <c r="A46" s="43"/>
-      <c r="B46" s="90" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
+      <c r="B46" s="91" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="91"/>
+      <c r="D46" s="91"/>
+      <c r="E46" s="91"/>
+      <c r="F46" s="91"/>
+      <c r="G46" s="91"/>
     </row>
     <row r="47" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A47" s="32"/>
@@ -4698,10 +4670,10 @@
         <v>1</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
@@ -4714,10 +4686,10 @@
         <v>2</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -4730,10 +4702,10 @@
         <v>3</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
@@ -4746,10 +4718,10 @@
         <v>4</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
@@ -4765,7 +4737,7 @@
         <v>22</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
@@ -4778,10 +4750,10 @@
         <v>6</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -4797,7 +4769,7 @@
         <v>119</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
@@ -4813,7 +4785,7 @@
         <v>23</v>
       </c>
       <c r="D54" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
@@ -4829,7 +4801,7 @@
         <v>24</v>
       </c>
       <c r="D55" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
@@ -4845,7 +4817,7 @@
         <v>26</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
@@ -4861,7 +4833,7 @@
         <v>25</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
@@ -4877,7 +4849,7 @@
         <v>27</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
@@ -4893,7 +4865,7 @@
         <v>28</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="22"/>
@@ -4909,7 +4881,7 @@
         <v>29</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
@@ -4925,7 +4897,7 @@
         <v>30</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E61" s="22"/>
       <c r="F61" s="22"/>
@@ -4941,7 +4913,7 @@
         <v>31</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E62" s="22"/>
       <c r="F62" s="22"/>
@@ -4958,14 +4930,14 @@
     </row>
     <row r="64" spans="1:7" s="44" customFormat="1" ht="16.5" customHeight="1">
       <c r="A64" s="43"/>
-      <c r="B64" s="90" t="s">
+      <c r="B64" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="C64" s="90"/>
+      <c r="C64" s="91"/>
       <c r="D64" s="72"/>
       <c r="E64" s="72"/>
-      <c r="F64" s="90"/>
-      <c r="G64" s="90"/>
+      <c r="F64" s="91"/>
+      <c r="G64" s="91"/>
     </row>
     <row r="65" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A65" s="32"/>
@@ -4976,7 +4948,7 @@
         <v>120</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E65" s="22"/>
       <c r="F65" s="22"/>
@@ -4992,7 +4964,7 @@
         <v>121</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E66" s="22"/>
       <c r="F66" s="22"/>
@@ -5005,10 +4977,10 @@
         <v>3</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E67" s="22"/>
       <c r="F67" s="22"/>
@@ -5021,10 +4993,10 @@
         <v>4</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E68" s="22"/>
       <c r="F68" s="22"/>
@@ -5041,11 +5013,11 @@
       </c>
       <c r="D69" s="22"/>
       <c r="E69" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F69" s="22"/>
-      <c r="G69" s="23" t="s">
-        <v>164</v>
+      <c r="G69" s="96" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="33" customFormat="1" ht="16.5">
@@ -5059,14 +5031,14 @@
     </row>
     <row r="71" spans="1:7" s="44" customFormat="1" ht="16.5" customHeight="1">
       <c r="A71" s="43"/>
-      <c r="B71" s="90" t="s">
+      <c r="B71" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="C71" s="90"/>
-      <c r="D71" s="90"/>
-      <c r="E71" s="90"/>
-      <c r="F71" s="90"/>
-      <c r="G71" s="90"/>
+      <c r="C71" s="91"/>
+      <c r="D71" s="91"/>
+      <c r="E71" s="91"/>
+      <c r="F71" s="91"/>
+      <c r="G71" s="91"/>
     </row>
     <row r="72" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A72" s="32"/>
@@ -5076,7 +5048,9 @@
       <c r="C72" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D72" s="22"/>
+      <c r="D72" s="22" t="s">
+        <v>153</v>
+      </c>
       <c r="E72" s="22"/>
       <c r="F72" s="22"/>
       <c r="G72" s="23"/>
@@ -5088,67 +5062,72 @@
         <v>2</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D73" s="22"/>
+        <v>125</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>153</v>
+      </c>
       <c r="E73" s="22"/>
       <c r="F73" s="22"/>
-      <c r="G73" s="23"/>
+      <c r="G73" s="96" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="74" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A74" s="32"/>
       <c r="B74" s="48">
-        <f t="shared" ref="B74:B75" si="5">B73+1</f>
+        <f t="shared" ref="B74" si="5">B73+1</f>
         <v>3</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D74" s="22"/>
+      <c r="D74" s="22" t="s">
+        <v>153</v>
+      </c>
       <c r="E74" s="22"/>
       <c r="F74" s="22"/>
       <c r="G74" s="23"/>
     </row>
     <row r="75" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="A75" s="32"/>
-      <c r="B75" s="48">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="C75" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="23"/>
-    </row>
-    <row r="76" spans="1:7" s="33" customFormat="1" ht="16.5">
-      <c r="A76" s="32"/>
-      <c r="B76" s="48"/>
-      <c r="C76" s="41"/>
-      <c r="D76" s="41"/>
-      <c r="E76" s="41"/>
-      <c r="F76" s="41"/>
-      <c r="G76" s="41"/>
-    </row>
-    <row r="77" spans="1:7" s="44" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A77" s="43"/>
-      <c r="B77" s="90" t="s">
+      <c r="B75" s="48"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="41"/>
+      <c r="F75" s="41"/>
+      <c r="G75" s="41"/>
+    </row>
+    <row r="76" spans="1:7" s="44" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A76" s="43"/>
+      <c r="B76" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="90"/>
-      <c r="D77" s="90"/>
-      <c r="E77" s="90"/>
-      <c r="F77" s="90"/>
-      <c r="G77" s="90"/>
+      <c r="C76" s="91"/>
+      <c r="D76" s="91"/>
+      <c r="E76" s="91"/>
+      <c r="F76" s="91"/>
+      <c r="G76" s="91"/>
+    </row>
+    <row r="77" spans="1:7" s="33" customFormat="1" ht="16.5">
+      <c r="B77" s="46">
+        <v>1</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="23"/>
     </row>
     <row r="78" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="B78" s="46">
-        <v>1</v>
+        <f>B77+1</f>
+        <v>2</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="22"/>
@@ -5157,11 +5136,11 @@
     </row>
     <row r="79" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="B79" s="46">
-        <f>B78+1</f>
-        <v>2</v>
+        <f t="shared" ref="B79:B83" si="6">B78+1</f>
+        <v>3</v>
       </c>
       <c r="C79" s="25" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="22"/>
@@ -5170,11 +5149,11 @@
     </row>
     <row r="80" spans="1:7" s="33" customFormat="1" ht="16.5">
       <c r="B80" s="46">
-        <f t="shared" ref="B80:B84" si="6">B79+1</f>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C80" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D80" s="22"/>
       <c r="E80" s="22"/>
@@ -5184,10 +5163,10 @@
     <row r="81" spans="2:7" s="33" customFormat="1" ht="16.5">
       <c r="B81" s="46">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="22"/>
@@ -5197,10 +5176,10 @@
     <row r="82" spans="2:7" s="33" customFormat="1" ht="16.5">
       <c r="B82" s="46">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C82" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="22"/>
@@ -5210,60 +5189,47 @@
     <row r="83" spans="2:7" s="33" customFormat="1" ht="16.5">
       <c r="B83" s="46">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C83" s="25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="22"/>
       <c r="F83" s="22"/>
       <c r="G83" s="23"/>
     </row>
-    <row r="84" spans="2:7" s="33" customFormat="1" ht="16.5">
-      <c r="B84" s="46">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="C84" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="23"/>
-    </row>
-    <row r="85" spans="2:7">
-      <c r="C85" s="31"/>
+    <row r="84" spans="2:7">
+      <c r="C84" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B3:C4"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="F33:G33"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
   </mergeCells>
-  <conditionalFormatting sqref="C85">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="C84">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IF(#REF!,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5277,7 +5243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -5299,16 +5265,16 @@
   <sheetData>
     <row r="1" spans="2:12" ht="67.5" customHeight="1"/>
     <row r="3" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="92"/>
+      <c r="D3" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88" t="s">
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="49"/>
@@ -5318,8 +5284,8 @@
       <c r="L3" s="49"/>
     </row>
     <row r="4" spans="2:12" ht="17.25">
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="53" t="s">
         <v>12</v>
       </c>
@@ -5329,7 +5295,7 @@
       <c r="F4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="88"/>
+      <c r="G4" s="92"/>
       <c r="H4" s="49"/>
       <c r="I4" s="49"/>
       <c r="J4" s="49"/>
@@ -5337,10 +5303,10 @@
       <c r="L4" s="49"/>
     </row>
     <row r="5" spans="2:12" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="90"/>
+      <c r="C5" s="91"/>
       <c r="D5" s="94"/>
       <c r="E5" s="94"/>
       <c r="F5" s="94"/>
@@ -5359,7 +5325,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
@@ -5381,7 +5347,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
@@ -5405,7 +5371,7 @@
       <c r="D8" s="38"/>
       <c r="E8" s="39"/>
       <c r="F8" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" s="40"/>
       <c r="H8" s="57"/>
@@ -5430,14 +5396,14 @@
       <c r="L9" s="49"/>
     </row>
     <row r="10" spans="2:12" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
       <c r="H10" s="54"/>
       <c r="I10" s="56"/>
       <c r="J10" s="56"/>
@@ -5449,10 +5415,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
@@ -5474,7 +5440,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
@@ -5497,11 +5463,11 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F13" s="39"/>
       <c r="G13" s="69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H13" s="57"/>
       <c r="I13" s="58">
@@ -5522,7 +5488,7 @@
       <c r="D14" s="38"/>
       <c r="E14" s="39"/>
       <c r="F14" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="57"/>
@@ -5547,14 +5513,14 @@
       <c r="L15" s="49"/>
     </row>
     <row r="16" spans="2:12" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="90"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="90"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="91"/>
       <c r="H16" s="54"/>
       <c r="I16" s="56"/>
       <c r="J16" s="56"/>
@@ -5591,18 +5557,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5632,22 +5598,22 @@
   <sheetData>
     <row r="1" spans="2:7" ht="67.5" customHeight="1"/>
     <row r="3" spans="2:7" ht="17.25">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="92"/>
+      <c r="D3" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88" t="s">
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="17.25">
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="53" t="s">
         <v>12</v>
       </c>
@@ -5657,13 +5623,13 @@
       <c r="F4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="88"/>
+      <c r="G4" s="92"/>
     </row>
     <row r="5" spans="2:7" ht="15.75">
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="90"/>
+      <c r="C5" s="91"/>
       <c r="D5" s="94"/>
       <c r="E5" s="94"/>
       <c r="F5" s="94"/>
@@ -5677,7 +5643,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E6" s="62"/>
       <c r="F6" s="62"/>
@@ -5692,11 +5658,11 @@
       </c>
       <c r="D7" s="61"/>
       <c r="E7" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F7" s="62"/>
       <c r="G7" s="63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="33" customFormat="1" ht="38.25" customHeight="1">
@@ -5704,15 +5670,15 @@
         <v>3</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="61"/>
       <c r="E8" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F8" s="62"/>
       <c r="G8" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="33" customFormat="1" ht="42" customHeight="1">
@@ -5724,11 +5690,11 @@
       </c>
       <c r="D9" s="61"/>
       <c r="E9" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F9" s="62"/>
       <c r="G9" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="2:7" s="33" customFormat="1" ht="16.5">
@@ -5740,10 +5706,10 @@
       <c r="G10" s="41"/>
     </row>
     <row r="11" spans="2:7" ht="19.5" customHeight="1">
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="90"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="95"/>
       <c r="E11" s="95"/>
       <c r="F11" s="95"/>
@@ -5757,7 +5723,7 @@
         <v>54</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="66"/>
       <c r="F12" s="66"/>
@@ -5771,7 +5737,7 @@
         <v>55</v>
       </c>
       <c r="D13" s="66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E13" s="66"/>
       <c r="F13" s="66"/>
@@ -5834,7 +5800,7 @@
         <v>60</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="66"/>
       <c r="F18" s="66"/>
@@ -5846,10 +5812,10 @@
         <v>8</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D19" s="66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E19" s="66"/>
       <c r="F19" s="66"/>
@@ -5864,14 +5830,14 @@
       <c r="G20" s="41"/>
     </row>
     <row r="21" spans="2:7" ht="21" customHeight="1">
-      <c r="B21" s="90" t="s">
+      <c r="B21" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
     </row>
     <row r="22" spans="2:7" s="33" customFormat="1" ht="16.5">
       <c r="B22" s="20">
@@ -5939,18 +5905,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>